<commit_message>
final update on Business rule verification
</commit_message>
<xml_diff>
--- a/VPSD/Stop_creation/Stops_Input.xlsx
+++ b/VPSD/Stop_creation/Stops_Input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Station_Name</t>
   </si>
@@ -51,18 +51,9 @@
     <t>Hubli BRTS</t>
   </si>
   <si>
-    <t>Vidya Nagar</t>
-  </si>
-  <si>
-    <t>Vidya Nagar,Hubli</t>
-  </si>
-  <si>
     <t>Stop_Name</t>
   </si>
   <si>
-    <t>Vidya Nagar 1</t>
-  </si>
-  <si>
     <t>Stop_Type</t>
   </si>
   <si>
@@ -75,17 +66,67 @@
     <t>Service_Type</t>
   </si>
   <si>
-    <t>City</t>
+    <t>VIDYA NAGAR</t>
+  </si>
+  <si>
+    <t>VIDYA NAGAR,HUBLI</t>
+  </si>
+  <si>
+    <t>VIDYA NAGAR 1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>User_Name</t>
+  </si>
+  <si>
+    <t>VPSD</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Vpsd@master@123</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://nechubli.com:5001</t>
+  </si>
+  <si>
+    <t>City,Suburban,All Stops</t>
+  </si>
+  <si>
+    <t>Color Code</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>VIDYA NAGAR BVB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,14 +148,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,110 +475,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" s="3">
+        <v>15.098768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>15.098768</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>75.989760000000004</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>